<commit_message>
Baud rate switch working (F2 key)
</commit_message>
<xml_diff>
--- a/MultiComp (VHDL Template)/Components/UART/Baud_Rate_Clock_DDS.xlsx
+++ b/MultiComp (VHDL Template)/Components/UART/Baud_Rate_Clock_DDS.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t xml:space="preserve">BAUD RATE</t>
   </si>
@@ -49,6 +49,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -132,8 +133,8 @@
   </sheetPr>
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="390" zoomScaleNormal="390" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -160,6 +161,9 @@
       <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
       <c r="F1" s="0" t="s">
         <v>4</v>
       </c>
@@ -219,14 +223,14 @@
         <v>307200</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>50000001</v>
+        <v>50000000</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>65537</v>
       </c>
       <c r="E4" s="0" t="n">
         <f aca="false">D4*B4/C4</f>
-        <v>402.659319946814</v>
+        <v>402.659328</v>
       </c>
       <c r="F4" s="0" t="n">
         <f aca="false">ROUND(E4,0)</f>
@@ -242,14 +246,14 @@
         <v>153600</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>50000002</v>
+        <v>50000000</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>65538</v>
       </c>
       <c r="E5" s="0" t="n">
         <f aca="false">D5*B5/C5</f>
-        <v>201.332727946691</v>
+        <v>201.332736</v>
       </c>
       <c r="F5" s="0" t="n">
         <f aca="false">ROUND(E5,0)</f>
@@ -265,14 +269,14 @@
         <v>76800</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>50000003</v>
+        <v>50000000</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>65539</v>
       </c>
       <c r="E6" s="0" t="n">
         <f aca="false">D6*B6/C6</f>
-        <v>100.667897959926</v>
+        <v>100.667904</v>
       </c>
       <c r="F6" s="0" t="n">
         <f aca="false">ROUND(E6,0)</f>
@@ -288,14 +292,14 @@
         <v>38400</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>50000004</v>
+        <v>50000000</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>65540</v>
       </c>
       <c r="E7" s="0" t="n">
         <f aca="false">D7*B7/C7</f>
-        <v>50.3347159732227</v>
+        <v>50.33472</v>
       </c>
       <c r="F7" s="0" t="n">
         <f aca="false">ROUND(E7,0)</f>
@@ -311,14 +315,14 @@
         <v>19200</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>50000005</v>
+        <v>50000000</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>65541</v>
       </c>
       <c r="E8" s="0" t="n">
         <f aca="false">D8*B8/C8</f>
-        <v>25.1677414832259</v>
+        <v>25.167744</v>
       </c>
       <c r="F8" s="0" t="n">
         <f aca="false">ROUND(E8,0)</f>
@@ -334,14 +338,14 @@
         <v>9600</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>50000006</v>
+        <v>50000000</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>65542</v>
       </c>
       <c r="E9" s="0" t="n">
         <f aca="false">D9*B9/C9</f>
-        <v>12.5840624899125</v>
+        <v>12.584064</v>
       </c>
       <c r="F9" s="0" t="n">
         <f aca="false">ROUND(E9,0)</f>
@@ -357,14 +361,14 @@
         <v>4800</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>50000007</v>
+        <v>50000000</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>65543</v>
       </c>
       <c r="E10" s="0" t="n">
         <f aca="false">D10*B10/C10</f>
-        <v>6.2921271191022</v>
+        <v>6.292128</v>
       </c>
       <c r="F10" s="0" t="n">
         <f aca="false">ROUND(E10,0)</f>

</xml_diff>